<commit_message>
Finished my own single function in EDA
</commit_message>
<xml_diff>
--- a/CH-176 Custom Grouping.xlsx
+++ b/CH-176 Custom Grouping.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EAB02-D531-49F9-8ACA-76C2348D35CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D10832-CB53-402F-A5E1-9E8F3BACA154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Question</t>
   </si>
@@ -369,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,11 +468,137 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -900,11 +1050,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C412C64-E88C-47F6-98DF-8E23E77E578F}" name="Table1" displayName="Table1" ref="B2:C27" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C412C64-E88C-47F6-98DF-8E23E77E578F}" name="Table1" displayName="Table1" ref="B2:C27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B2:C27" xr:uid="{6C412C64-E88C-47F6-98DF-8E23E77E578F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B5E0013D-3A3B-4DE2-B37A-1EA6163FBB07}" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{89A7122A-0D05-4FFD-A71D-A1FD6E9DEB02}" name="Quantity" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B5E0013D-3A3B-4DE2-B37A-1EA6163FBB07}" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{89A7122A-0D05-4FFD-A71D-A1FD6E9DEB02}" name="Quantity" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6671F958-0602-4CF8-A60F-1B7F64D0B91D}" name="Table13" displayName="Table13" ref="B2:C27" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="B2:C27" xr:uid="{6C412C64-E88C-47F6-98DF-8E23E77E578F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{57199793-B68A-46FE-A3C2-18B1111E23C5}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3FFE6C19-3A7F-42E5-A7B8-6A973CD01CA4}" name="Quantity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1543,4 +1704,460 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592416B0-7F98-4DE5-8D61-A84788C084BC}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="E1"/>
+      <c r="F1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="39"/>
+      <c r="I1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="27">
+        <v>47</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3"/>
+      <c r="F3" s="17">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14">
+        <v>217</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="27">
+        <v>62</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4"/>
+      <c r="F4" s="18">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15">
+        <v>253</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22">
+        <f>B4+1</f>
+        <v>45294</v>
+      </c>
+      <c r="C5" s="27">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5"/>
+      <c r="F5" s="19">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12">
+        <v>334</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="22">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="27">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="11">
+        <v>484</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="22">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="27">
+        <v>55</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7"/>
+      <c r="F7" s="21">
+        <v>5</v>
+      </c>
+      <c r="G7" s="16">
+        <v>438</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="28">
+        <v>65</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5"/>
+      <c r="G8"/>
+      <c r="H8" s="10"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="28">
+        <v>72</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5"/>
+      <c r="G9"/>
+      <c r="H9" s="10"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="23">
+        <v>45301</v>
+      </c>
+      <c r="C10" s="28">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="5"/>
+      <c r="G10"/>
+      <c r="H10" s="10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="23">
+        <v>45307</v>
+      </c>
+      <c r="C11" s="28">
+        <v>61</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11"/>
+      <c r="H11" s="10"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23">
+        <v>45308</v>
+      </c>
+      <c r="C12" s="28">
+        <v>25</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="5"/>
+      <c r="G12"/>
+      <c r="H12" s="6" t="str" cm="1">
+        <f t="array" ref="H12:I17">_xlfn.LET(
+_xlpm.g, _xlfn.SEQUENCE(25,1,0,1),
+_xlpm.gg, QUOTIENT(_xlpm.g,5)+1,
+_xlfn.VSTACK({"Group","Quantity"},_xlfn.GROUPBY(_xlpm.gg,Table13[Quantity],_xleta.SUM,,0))
+)</f>
+        <v>Group</v>
+      </c>
+      <c r="I12" s="13" t="str">
+        <v>Quantity</v>
+      </c>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="24">
+        <v>45309</v>
+      </c>
+      <c r="C13" s="29">
+        <v>55</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="H13" s="17">
+        <v>1</v>
+      </c>
+      <c r="I13" s="14">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="24">
+        <v>45310</v>
+      </c>
+      <c r="C14" s="29">
+        <v>52</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="H14" s="18">
+        <v>2</v>
+      </c>
+      <c r="I14" s="15">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="24">
+        <v>45314</v>
+      </c>
+      <c r="C15" s="29">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="H15" s="19">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="24">
+        <v>45325</v>
+      </c>
+      <c r="C16" s="29">
+        <v>99</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="H16" s="20">
+        <v>4</v>
+      </c>
+      <c r="I16" s="11">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="24">
+        <v>45330</v>
+      </c>
+      <c r="C17" s="29">
+        <v>110</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="H17" s="21">
+        <v>5</v>
+      </c>
+      <c r="I17" s="16">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="25">
+        <v>45331</v>
+      </c>
+      <c r="C18" s="30">
+        <v>106</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="25">
+        <v>45333</v>
+      </c>
+      <c r="C19" s="30">
+        <v>103</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="25">
+        <v>45334</v>
+      </c>
+      <c r="C20" s="30">
+        <v>100</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="1"/>
+      <c r="H20" s="40"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="25">
+        <v>45335</v>
+      </c>
+      <c r="C21" s="30">
+        <v>85</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="1"/>
+      <c r="H21" s="40"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="25">
+        <v>45336</v>
+      </c>
+      <c r="C22" s="30">
+        <v>90</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="1"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="26">
+        <v>45337</v>
+      </c>
+      <c r="C23" s="31">
+        <v>80</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="1"/>
+      <c r="H23" s="40"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="26">
+        <v>45342</v>
+      </c>
+      <c r="C24" s="31">
+        <v>75</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="1"/>
+      <c r="H24" s="40"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="26">
+        <v>45343</v>
+      </c>
+      <c r="C25" s="31">
+        <v>84</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="1"/>
+      <c r="H25" s="40"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="26">
+        <v>45344</v>
+      </c>
+      <c r="C26" s="31">
+        <v>94</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="32">
+        <v>45346</v>
+      </c>
+      <c r="C27" s="33">
+        <v>105</v>
+      </c>
+      <c r="H27" s="41"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H28" s="41"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H29" s="41"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H30" s="41"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H31" s="41"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H32" s="41"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="41"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="41"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="41"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>